<commit_message>
Se agregan las pruebas de reconocimiento y se ajusta la estratégía
</commit_message>
<xml_diff>
--- a/Pruebas exploratorias/inventario-pruebas-exploratorias.xlsx
+++ b/Pruebas exploratorias/inventario-pruebas-exploratorias.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://interpublic-my.sharepoint.com/personal/juan_oliveros_initiative_com/Documents/MAESTRIA UNIANDES/MASTER TRACK 2/AUTOMATIZACION DE PRUEBAS/WEEK 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PA\semana5PruebasAutomatizadas\Pruebas exploratorias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{164BC5CD-DB63-412C-A93C-08D7A71492B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BCAC0675-00C9-4CFD-B71F-99B1F1BC14D0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3115509-80AD-4741-AAAB-4ECBD1A854A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Lists" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Escenarios PE'!$A$1:$J$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Escenarios PE'!$A$1:$J$40</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
   <si>
     <t>Funcionalidad</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Ambiente de pruebas</t>
-  </si>
-  <si>
-    <t>&lt;Versión y hash del commit en el repo&gt;</t>
   </si>
   <si>
     <t>Escenarios de pruebas ejecutados</t>
@@ -102,18 +99,6 @@
   <si>
     <t>Tipo de escenario
 (Positivo, Negativo, Mix)</t>
-  </si>
-  <si>
-    <t>P001</t>
-  </si>
-  <si>
-    <t>P002</t>
-  </si>
-  <si>
-    <t>P003</t>
-  </si>
-  <si>
-    <t>P004</t>
   </si>
   <si>
     <t>P005</t>
@@ -142,30 +127,6 @@
     <t>En operación normal</t>
   </si>
   <si>
-    <t>https://vimeo.com/506729301</t>
-  </si>
-  <si>
-    <t>https://vimeo.com/506729792</t>
-  </si>
-  <si>
-    <t>Borrador - crear un post</t>
-  </si>
-  <si>
-    <t>Borrador - eliminar un post</t>
-  </si>
-  <si>
-    <t>Borrador - modificar un post</t>
-  </si>
-  <si>
-    <t>https://vimeo.com/506730169</t>
-  </si>
-  <si>
-    <t>Borrador - filtrar un post</t>
-  </si>
-  <si>
-    <t>https://vimeo.com/506730574</t>
-  </si>
-  <si>
     <t>Programar - un post</t>
   </si>
   <si>
@@ -196,18 +157,6 @@
     <t>https://vimeo.com/506739917</t>
   </si>
   <si>
-    <t>https://vimeo.com/506740184/47c36f9f98</t>
-  </si>
-  <si>
-    <t>P001-2</t>
-  </si>
-  <si>
-    <t>P003-2</t>
-  </si>
-  <si>
-    <t>P004-2</t>
-  </si>
-  <si>
     <t>P005-2</t>
   </si>
   <si>
@@ -217,12 +166,6 @@
     <t>P007-2</t>
   </si>
   <si>
-    <t>https://vimeo.com/506740972/5bd683c342</t>
-  </si>
-  <si>
-    <t>https://vimeo.com/506741331/5850e066e4</t>
-  </si>
-  <si>
     <t>https://vimeo.com/506741829</t>
   </si>
   <si>
@@ -338,13 +281,16 @@
   </si>
   <si>
     <t>https://vimeo.com/506774423/65a2e645cc</t>
+  </si>
+  <si>
+    <t>3.0.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -375,6 +321,14 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -402,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -462,24 +416,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -494,8 +436,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -524,8 +464,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -547,13 +489,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1923676</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>56030</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>373530</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>279455</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -859,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J42"/>
+  <dimension ref="B1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="68" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -890,17 +832,17 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -917,46 +859,46 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="19"/>
+      <c r="C4" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
+      <c r="C5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="2:10" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="16"/>
+      <c r="C6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
@@ -970,24 +912,24 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>4</v>
@@ -996,868 +938,682 @@
         <v>0</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="6">
         <v>44227</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C11" s="6">
         <v>44227</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="J11" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="9">
-        <v>44227</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" s="8"/>
+      <c r="B12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="6">
+        <v>44227</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C13" s="6">
         <v>44227</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>39</v>
+        <v>26</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="C14" s="6">
         <v>44227</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>39</v>
+        <v>26</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C15" s="6">
         <v>44227</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>41</v>
+        <v>26</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C16" s="6">
         <v>44227</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>41</v>
+        <v>26</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="C17" s="6">
         <v>44227</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>43</v>
+        <v>26</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C18" s="6">
         <v>44227</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>43</v>
+        <v>26</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C19" s="6">
         <v>44227</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C20" s="6">
         <v>44227</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="5" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="C21" s="6">
         <v>44227</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>47</v>
+        <v>26</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C22" s="6">
         <v>44227</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>47</v>
+        <v>26</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C23" s="6">
         <v>44227</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>49</v>
+        <v>26</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="6">
         <v>44227</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>49</v>
+        <v>26</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C25" s="6">
         <v>44227</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="6">
+        <v>44227</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="6">
-        <v>44227</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="F26" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J26" s="5"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C27" s="6">
         <v>44227</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C28" s="6">
         <v>44227</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="J28" s="5"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C29" s="6">
         <v>44227</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="J29" s="5"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C30" s="6">
         <v>44227</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C31" s="6">
         <v>44227</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="6">
-        <v>44227</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="J32" s="5"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="6">
-        <v>44227</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J33" s="5"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="6">
-        <v>44227</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="6">
-        <v>44227</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C36" s="6">
-        <v>44227</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I36" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="6">
-        <v>44227</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="6">
-        <v>44227</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B10:J38">
-    <sortCondition ref="B10:B38"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B10:J31">
+    <sortCondition ref="B10:B31"/>
   </sortState>
   <mergeCells count="6">
     <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="B8:J8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="J11" r:id="rId1" xr:uid="{7B12B707-E752-479A-80F9-A589824109A2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -1865,13 +1621,13 @@
           <x14:formula1>
             <xm:f>Lists!$B$4:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F10:F40</xm:sqref>
+          <xm:sqref>F10:F33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Lists!$B$8:$B$10</xm:f>
           </x14:formula1>
-          <xm:sqref>G10:G40</xm:sqref>
+          <xm:sqref>G10:G33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1895,33 +1651,33 @@
   <sheetData>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agregan más pruebas
</commit_message>
<xml_diff>
--- a/Pruebas exploratorias/inventario-pruebas-exploratorias.xlsx
+++ b/Pruebas exploratorias/inventario-pruebas-exploratorias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PA\semana5PruebasAutomatizadas\Pruebas exploratorias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3115509-80AD-4741-AAAB-4ECBD1A854A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5DCF73-6D9E-4217-B93C-0A1AB17D6191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,7 +283,7 @@
     <t>https://vimeo.com/506774423/65a2e645cc</t>
   </si>
   <si>
-    <t>3.0.0</t>
+    <t>3.3.0</t>
   </si>
 </sst>
 </file>
@@ -437,6 +437,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -464,7 +465,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -804,7 +804,7 @@
   <dimension ref="B1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="68" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="C6" sqref="C6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -832,17 +832,17 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
@@ -859,46 +859,46 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="2:10" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="2:10" ht="81.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
@@ -912,17 +912,17 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="2:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="2:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -1005,7 +1005,7 @@
       <c r="I11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="18" t="s">
+      <c r="J11" s="9" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1583,17 +1583,17 @@
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="2:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B10:J31">

</xml_diff>